<commit_message>
added a semicolon in the add post test data, test fails
</commit_message>
<xml_diff>
--- a/src/data/testData.xlsx
+++ b/src/data/testData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="232" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -123,7 +123,7 @@
     <t>@;':”</t>
   </si>
   <si>
-    <t>Characters</t>
+    <t>Characters;</t>
   </si>
   <si>
     <t>Old Password</t>
@@ -548,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -702,7 +702,7 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>